<commit_message>
batch execution elapsed time + fixes
</commit_message>
<xml_diff>
--- a/results/aggr_usu_test_results.xlsx
+++ b/results/aggr_usu_test_results.xlsx
@@ -486,11 +486,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Nombres: Santiago Alejandro
+          <t>Nombres: Martín Andrés
 Apellidos: Ramírez González
-Tipo Doc: C.C.
-Num Doc: 67890123
-Roles: ['Gestor 2', 'Gestor 1', 'Administrador']</t>
+Tipo Doc: Pasaporte
+Num Doc: 67890123 - 1681735068
+Roles: ['Solicitante', 'Gestor 1', 'Recepción', 'Gestor 2', 'Administrador']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -525,11 +525,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Nombres: Santiago Alejandro
+          <t>Nombres: Martín Andrés
 Apellidos: Ramírez González
-Tipo Doc: C.C.
-Num Doc: 67890123
-Roles: ['Gestor 2', 'Gestor 1', 'Administrador']</t>
+Tipo Doc: Pasaporte
+Num Doc: 67890123 - 1681735068
+Roles: ['Solicitante', 'Gestor 1', 'Recepción', 'Gestor 2', 'Administrador']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -539,12 +539,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>SI : se encontró un resultado en Usuarios que coincide con [['gamerboy42', 'Gestor 2 Gestor 1 Administrador']]</t>
+          <t>NO : no se encontraron resultados en Usuarios para ['gamerboy42 - 1681735068', 'Solicitante Gestor 1 Recepción Gestor 2 Administrador']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>PASSED</t>
+          <t>FAILED</t>
         </is>
       </c>
     </row>
@@ -564,11 +564,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Nombres: Santiago Alejandro
+          <t>Nombres: Martín Andrés
 Apellidos: Ramírez González
-Tipo Doc: C.C.
-Num Doc: 67890123
-Roles: ['Gestor 2', 'Gestor 1', 'Administrador']</t>
+Tipo Doc: Pasaporte
+Num Doc: 67890123 - 1681735068
+Roles: ['Solicitante', 'Gestor 1', 'Recepción', 'Gestor 2', 'Administrador']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -578,7 +578,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>SI : ['gamerboy42', 'Santiago Alejandro', 'Ramírez González', 'C.C.', '67890123', True, ['Administrador', 'Gestor 1', 'Gestor 2']] y ['gamerboy42', 'Santiago Alejandro', 'Ramírez González', 'C.C.', '67890123', True, ['Administrador', 'Gestor 1', 'Gestor 2']] coinciden</t>
+          <t>SI : ['gamerboy42 - 1681735068', 'Martín Andrés', 'Ramírez González', 'Pasaporte', '67890123 - 1681735068', True, ['Administrador', 'Gestor 1', 'Gestor 2', 'Recepción', 'Solicitante']] y ['gamerboy42 - 1681735068', 'Martín Andrés', 'Ramírez González', 'Pasaporte', '67890123 - 1681735068', True, ['Administrador', 'Gestor 1', 'Gestor 2', 'Recepción', 'Solicitante']] coinciden</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -603,11 +603,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: García Pérez
+          <t>Nombres: Ana Isabel
+Apellidos: Martínez Sánchez
 Tipo Doc: Cédula de Extranjería
-Num Doc: FG789012
-Roles: ['Gestor 2', 'Recepción', 'Solicitante']</t>
+Num Doc: FG789012 - 1681735110
+Roles: ['Gestor 2', 'Recepción']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -642,11 +642,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: García Pérez
+          <t>Nombres: Ana Isabel
+Apellidos: Martínez Sánchez
 Tipo Doc: Cédula de Extranjería
-Num Doc: FG789012
-Roles: ['Gestor 2', 'Recepción', 'Solicitante']</t>
+Num Doc: FG789012 - 1681735110
+Roles: ['Gestor 2', 'Recepción']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -656,12 +656,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>SI : se encontró un resultado en Usuarios que coincide con [['mysticalunicorn88', 'Gestor 2 Recepción Solicitante']]</t>
+          <t>NO : no se encontraron resultados en Usuarios para ['mysticalunicorn88 - 1681735110', 'Gestor 2 Recepción']</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>PASSED</t>
+          <t>FAILED</t>
         </is>
       </c>
     </row>
@@ -681,11 +681,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: García Pérez
+          <t>Nombres: Ana Isabel
+Apellidos: Martínez Sánchez
 Tipo Doc: Cédula de Extranjería
-Num Doc: FG789012
-Roles: ['Gestor 2', 'Recepción', 'Solicitante']</t>
+Num Doc: FG789012 - 1681735110
+Roles: ['Gestor 2', 'Recepción']</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>SI : ['mysticalunicorn88', 'Martín Andrés', 'García Pérez', 'Cédula de Extranjería', 'FG789012', True, ['Gestor 2', 'Recepción', 'Solicitante']] y ['mysticalunicorn88', 'Martín Andrés', 'García Pérez', 'Cédula de Extranjería', 'FG789012', True, ['Gestor 2', 'Recepción', 'Solicitante']] coinciden</t>
+          <t>SI : ['mysticalunicorn88 - 1681735110', 'Ana Isabel', 'Martínez Sánchez', 'Cédula de Extranjería', 'FG789012 - 1681735110', True, ['Gestor 2', 'Recepción']] y ['mysticalunicorn88 - 1681735110', 'Ana Isabel', 'Martínez Sánchez', 'Cédula de Extranjería', 'FG789012 - 1681735110', True, ['Gestor 2', 'Recepción']] coinciden</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -720,11 +720,11 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Nombres: Sofía Elena
-Apellidos: Castro Ruiz
+          <t>Nombres: Martín Andrés
+Apellidos: Martínez Sánchez
 Tipo Doc: T.I.
-Num Doc: 1234567A
-Roles: ['Gestor 1', 'Recepción', 'Solicitante', 'Administrador']</t>
+Num Doc: 1234567A - 1681735152
+Roles: ['Recepción', 'Gestor 1', 'Administrador', 'Gestor 2', 'Solicitante']</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -759,11 +759,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Nombres: Sofía Elena
-Apellidos: Castro Ruiz
+          <t>Nombres: Martín Andrés
+Apellidos: Martínez Sánchez
 Tipo Doc: T.I.
-Num Doc: 1234567A
-Roles: ['Gestor 1', 'Recepción', 'Solicitante', 'Administrador']</t>
+Num Doc: 1234567A - 1681735152
+Roles: ['Recepción', 'Gestor 1', 'Administrador', 'Gestor 2', 'Solicitante']</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -773,7 +773,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>SI : se encontró un resultado en Usuarios que coincide con [['lovetoswim99', 'Gestor 1 Recepción Solicitante Administrador']]</t>
+          <t>SI : se encontró un resultado en Usuarios que coincide con [['lovetoswim99 - 1681735152', 'Recepción Gestor 1 Administrador Gestor 2 Solicitante']]</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -798,11 +798,11 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Nombres: Sofía Elena
-Apellidos: Castro Ruiz
+          <t>Nombres: Martín Andrés
+Apellidos: Martínez Sánchez
 Tipo Doc: T.I.
-Num Doc: 1234567A
-Roles: ['Gestor 1', 'Recepción', 'Solicitante', 'Administrador']</t>
+Num Doc: 1234567A - 1681735152
+Roles: ['Recepción', 'Gestor 1', 'Administrador', 'Gestor 2', 'Solicitante']</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -812,7 +812,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>SI : ['lovetoswim99', 'Sofía Elena', 'Castro Ruiz', 'T.I.', '1234567A', True, ['Administrador', 'Gestor 1', 'Recepción', 'Solicitante']] y ['lovetoswim99', 'Sofía Elena', 'Castro Ruiz', 'T.I.', '1234567A', True, ['Administrador', 'Gestor 1', 'Recepción', 'Solicitante']] coinciden</t>
+          <t>SI : ['lovetoswim99 - 1681735152', 'Martín Andrés', 'Martínez Sánchez', 'T.I.', '1234567A - 1681735152', True, ['Administrador', 'Gestor 1', 'Gestor 2', 'Recepción', 'Solicitante']] y ['lovetoswim99 - 1681735152', 'Martín Andrés', 'Martínez Sánchez', 'T.I.', '1234567A - 1681735152', True, ['Administrador', 'Gestor 1', 'Gestor 2', 'Recepción', 'Solicitante']] coinciden</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -837,11 +837,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Nombres: Valentina Victoria
-Apellidos: Martínez Sánchez
-Tipo Doc: Cédula de Extranjería
-Num Doc: 4567890B
-Roles: ['Recepción']</t>
+          <t>Nombres: Martín Andrés
+Apellidos: Gómez Rodríguez
+Tipo Doc: C.C.
+Num Doc: 4567890B - 1681735192
+Roles: ['Solicitante', 'Gestor 2', 'Administrador', 'Recepción']</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -876,11 +876,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Nombres: Valentina Victoria
-Apellidos: Martínez Sánchez
-Tipo Doc: Cédula de Extranjería
-Num Doc: 4567890B
-Roles: ['Recepción']</t>
+          <t>Nombres: Martín Andrés
+Apellidos: Gómez Rodríguez
+Tipo Doc: C.C.
+Num Doc: 4567890B - 1681735192
+Roles: ['Solicitante', 'Gestor 2', 'Administrador', 'Recepción']</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -890,7 +890,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>SI : se encontró un resultado en Usuarios que coincide con [['hikingfanatic33', 'Recepción']]</t>
+          <t>SI : se encontró un resultado en Usuarios que coincide con [['hikingfanatic33 - 1681735192', 'Solicitante Gestor 2 Administrador Recepción']]</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -915,11 +915,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Nombres: Valentina Victoria
-Apellidos: Martínez Sánchez
-Tipo Doc: Cédula de Extranjería
-Num Doc: 4567890B
-Roles: ['Recepción']</t>
+          <t>Nombres: Martín Andrés
+Apellidos: Gómez Rodríguez
+Tipo Doc: C.C.
+Num Doc: 4567890B - 1681735192
+Roles: ['Solicitante', 'Gestor 2', 'Administrador', 'Recepción']</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>SI : ['hikingfanatic33', 'Valentina Victoria', 'Martínez Sánchez', 'Cédula de Extranjería', '4567890B', True, ['Recepción']] y ['hikingfanatic33', 'Valentina Victoria', 'Martínez Sánchez', 'Cédula de Extranjería', '4567890B', True, ['Recepción']] coinciden</t>
+          <t>SI : ['hikingfanatic33 - 1681735192', 'Martín Andrés', 'Gómez Rodríguez', 'C.C.', '4567890B - 1681735192', True, ['Administrador', 'Gestor 2', 'Recepción', 'Solicitante']] y ['hikingfanatic33 - 1681735192', 'Martín Andrés', 'Gómez Rodríguez', 'C.C.', '4567890B - 1681735192', True, ['Administrador', 'Gestor 2', 'Recepción', 'Solicitante']] coinciden</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -954,11 +954,11 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: Martínez Sánchez
-Tipo Doc: Cédula de Extranjería
-Num Doc: 8901234C
-Roles: ['Gestor 1', 'Recepción']</t>
+          <t>Nombres: Ana Isabel
+Apellidos: García Pérez
+Tipo Doc: Pasaporte
+Num Doc: 8901234C - 1681735237
+Roles: ['Recepción']</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -993,11 +993,11 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: Martínez Sánchez
-Tipo Doc: Cédula de Extranjería
-Num Doc: 8901234C
-Roles: ['Gestor 1', 'Recepción']</t>
+          <t>Nombres: Ana Isabel
+Apellidos: García Pérez
+Tipo Doc: Pasaporte
+Num Doc: 8901234C - 1681735237
+Roles: ['Recepción']</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1007,7 +1007,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>SI : se encontró un resultado en Usuarios que coincide con [['teadrinker12', 'Gestor 1 Recepción']]</t>
+          <t>SI : se encontró un resultado en Usuarios que coincide con [['teadrinker12 - 1681735237', 'Recepción']]</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1032,11 +1032,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: Martínez Sánchez
-Tipo Doc: Cédula de Extranjería
-Num Doc: 8901234C
-Roles: ['Gestor 1', 'Recepción']</t>
+          <t>Nombres: Ana Isabel
+Apellidos: García Pérez
+Tipo Doc: Pasaporte
+Num Doc: 8901234C - 1681735237
+Roles: ['Recepción']</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>SI : ['teadrinker12', 'Martín Andrés', 'Martínez Sánchez', 'Cédula de Extranjería', '8901234C', True, ['Gestor 1', 'Recepción']] y ['teadrinker12', 'Martín Andrés', 'Martínez Sánchez', 'Cédula de Extranjería', '8901234C', True, ['Gestor 1', 'Recepción']] coinciden</t>
+          <t>SI : ['teadrinker12 - 1681735237', 'Ana Isabel', 'García Pérez', 'Pasaporte', '8901234C - 1681735237', True, ['Recepción']] y ['teadrinker12 - 1681735237', 'Ana Isabel', 'García Pérez', 'Pasaporte', '8901234C - 1681735237', True, ['Recepción']] coinciden</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1071,11 +1071,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: Gómez Rodríguez
-Tipo Doc: Pasaporte
-Num Doc: 2345678D
-Roles: ['Gestor 2', 'Administrador', 'Gestor 1', 'Solicitante']</t>
+          <t>Nombres: Ana Isabel
+Apellidos: Martínez Sánchez
+Tipo Doc: Cédula de Extranjería
+Num Doc: 2345678D - 1681735278
+Roles: ['Solicitante']</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1110,11 +1110,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: Gómez Rodríguez
-Tipo Doc: Pasaporte
-Num Doc: 2345678D
-Roles: ['Gestor 2', 'Administrador', 'Gestor 1', 'Solicitante']</t>
+          <t>Nombres: Ana Isabel
+Apellidos: Martínez Sánchez
+Tipo Doc: Cédula de Extranjería
+Num Doc: 2345678D - 1681735278
+Roles: ['Solicitante']</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>SI : se encontró un resultado en Usuarios que coincide con [['familyman77', 'Gestor 2 Administrador Gestor 1 Solicitante']]</t>
+          <t>SI : se encontró un resultado en Usuarios que coincide con [['familyman77 - 1681735278', 'Solicitante']]</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1149,11 +1149,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: Gómez Rodríguez
-Tipo Doc: Pasaporte
-Num Doc: 2345678D
-Roles: ['Gestor 2', 'Administrador', 'Gestor 1', 'Solicitante']</t>
+          <t>Nombres: Ana Isabel
+Apellidos: Martínez Sánchez
+Tipo Doc: Cédula de Extranjería
+Num Doc: 2345678D - 1681735278
+Roles: ['Solicitante']</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>SI : ['familyman77', 'Martín Andrés', 'Gómez Rodríguez', 'Pasaporte', '2345678D', True, ['Administrador', 'Gestor 1', 'Gestor 2', 'Solicitante']] y ['familyman77', 'Martín Andrés', 'Gómez Rodríguez', 'Pasaporte', '2345678D', True, ['Administrador', 'Gestor 1', 'Gestor 2', 'Solicitante']] coinciden</t>
+          <t>SI : ['familyman77 - 1681735278', 'Ana Isabel', 'Martínez Sánchez', 'Cédula de Extranjería', '2345678D - 1681735278', True, ['Solicitante']] y ['familyman77 - 1681735278', 'Ana Isabel', 'Martínez Sánchez', 'Cédula de Extranjería', '2345678D - 1681735278', True, ['Solicitante']] coinciden</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1188,11 +1188,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Nombres: Valentina Victoria
+          <t>Nombres: Santiago Alejandro
 Apellidos: Castro Ruiz
-Tipo Doc: Pasaporte
-Num Doc: 5678901E
-Roles: ['Administrador', 'Solicitante', 'Gestor 1', 'Recepción', 'Gestor 2']</t>
+Tipo Doc: C.C.
+Num Doc: 5678901E - 1681735319
+Roles: ['Administrador', 'Recepción', 'Gestor 2']</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1227,11 +1227,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Nombres: Valentina Victoria
+          <t>Nombres: Santiago Alejandro
 Apellidos: Castro Ruiz
-Tipo Doc: Pasaporte
-Num Doc: 5678901E
-Roles: ['Administrador', 'Solicitante', 'Gestor 1', 'Recepción', 'Gestor 2']</t>
+Tipo Doc: C.C.
+Num Doc: 5678901E - 1681735319
+Roles: ['Administrador', 'Recepción', 'Gestor 2']</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1241,12 +1241,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>SI : se encontró un resultado en Usuarios que coincide con [['doglover88', 'Administrador Solicitante Gestor 1 Recepción Gestor 2']]</t>
+          <t>NO : no se encontraron resultados en Usuarios para ['doglover88 - 1681735319', 'Administrador Recepción Gestor 2']</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>PASSED</t>
+          <t>FAILED</t>
         </is>
       </c>
     </row>
@@ -1266,11 +1266,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Nombres: Valentina Victoria
+          <t>Nombres: Santiago Alejandro
 Apellidos: Castro Ruiz
-Tipo Doc: Pasaporte
-Num Doc: 5678901E
-Roles: ['Administrador', 'Solicitante', 'Gestor 1', 'Recepción', 'Gestor 2']</t>
+Tipo Doc: C.C.
+Num Doc: 5678901E - 1681735319
+Roles: ['Administrador', 'Recepción', 'Gestor 2']</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1280,7 +1280,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>SI : ['doglover88', 'Valentina Victoria', 'Castro Ruiz', 'Pasaporte', '5678901E', True, ['Administrador', 'Gestor 1', 'Gestor 2', 'Recepción', 'Solicitante']] y ['doglover88', 'Valentina Victoria', 'Castro Ruiz', 'Pasaporte', '5678901E', True, ['Administrador', 'Gestor 1', 'Gestor 2', 'Recepción', 'Solicitante']] coinciden</t>
+          <t>SI : ['doglover88 - 1681735319', 'Santiago Alejandro', 'Castro Ruiz', 'C.C.', '5678901E - 1681735319', True, ['Administrador', 'Gestor 2', 'Recepción']] y ['doglover88 - 1681735319', 'Santiago Alejandro', 'Castro Ruiz', 'C.C.', '5678901E - 1681735319', True, ['Administrador', 'Gestor 2', 'Recepción']] coinciden</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1305,11 +1305,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Nombres: Santiago Alejandro
-Apellidos: Gómez Rodríguez
-Tipo Doc: C.C.
-Num Doc: 9012345F
-Roles: ['Gestor 2', 'Administrador']</t>
+          <t>Nombres: Valentina Victoria
+Apellidos: Martínez Sánchez
+Tipo Doc: Cédula de Extranjería
+Num Doc: 9012345F - 1681735360
+Roles: ['Gestor 1', 'Recepción', 'Solicitante']</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1344,11 +1344,11 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Nombres: Santiago Alejandro
-Apellidos: Gómez Rodríguez
-Tipo Doc: C.C.
-Num Doc: 9012345F
-Roles: ['Gestor 2', 'Administrador']</t>
+          <t>Nombres: Valentina Victoria
+Apellidos: Martínez Sánchez
+Tipo Doc: Cédula de Extranjería
+Num Doc: 9012345F - 1681735360
+Roles: ['Gestor 1', 'Recepción', 'Solicitante']</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>SI : se encontró un resultado en Usuarios que coincide con [['catlady44', 'Gestor 2 Administrador']]</t>
+          <t>SI : se encontró un resultado en Usuarios que coincide con [['catlady44 - 1681735360', 'Gestor 1 Recepción Solicitante']]</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1383,11 +1383,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Nombres: Santiago Alejandro
-Apellidos: Gómez Rodríguez
-Tipo Doc: C.C.
-Num Doc: 9012345F
-Roles: ['Gestor 2', 'Administrador']</t>
+          <t>Nombres: Valentina Victoria
+Apellidos: Martínez Sánchez
+Tipo Doc: Cédula de Extranjería
+Num Doc: 9012345F - 1681735360
+Roles: ['Gestor 1', 'Recepción', 'Solicitante']</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>SI : ['catlady44', 'Santiago Alejandro', 'Gómez Rodríguez', 'C.C.', '9012345F', True, ['Administrador', 'Gestor 2']] y ['catlady44', 'Santiago Alejandro', 'Gómez Rodríguez', 'C.C.', '9012345F', True, ['Administrador', 'Gestor 2']] coinciden</t>
+          <t>SI : ['catlady44 - 1681735360', 'Valentina Victoria', 'Martínez Sánchez', 'Cédula de Extranjería', '9012345F - 1681735360', True, ['Gestor 1', 'Recepción', 'Solicitante']] y ['catlady44 - 1681735360', 'Valentina Victoria', 'Martínez Sánchez', 'Cédula de Extranjería', '9012345F - 1681735360', True, ['Gestor 1', 'Recepción', 'Solicitante']] coinciden</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1422,11 +1422,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: Martínez Sánchez
-Tipo Doc: Cédula de Extranjería
-Num Doc: CD567890
-Roles: ['Gestor 2', 'Solicitante', 'Recepción']</t>
+          <t>Nombres: Sofía Elena
+Apellidos: Martínez Sánchez
+Tipo Doc: T.I.
+Num Doc: CD567890 - 1681735403
+Roles: ['Solicitante', 'Recepción']</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1461,11 +1461,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: Martínez Sánchez
-Tipo Doc: Cédula de Extranjería
-Num Doc: CD567890
-Roles: ['Gestor 2', 'Solicitante', 'Recepción']</t>
+          <t>Nombres: Sofía Elena
+Apellidos: Martínez Sánchez
+Tipo Doc: T.I.
+Num Doc: CD567890 - 1681735403
+Roles: ['Solicitante', 'Recepción']</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1475,12 +1475,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>SI : se encontró un resultado en Usuarios que coincide con [['birdwatcher22', 'Gestor 2 Solicitante Recepción']]</t>
+          <t>NO : no se encontraron resultados en Usuarios para ['birdwatcher22 - 1681735403', 'Solicitante Recepción']</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>PASSED</t>
+          <t>FAILED</t>
         </is>
       </c>
     </row>
@@ -1500,26 +1500,26 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Nombres: Martín Andrés
-Apellidos: Martínez Sánchez
-Tipo Doc: Cédula de Extranjería
-Num Doc: CD567890
-Roles: ['Gestor 2', 'Solicitante', 'Recepción']</t>
+          <t>Nombres: Sofía Elena
+Apellidos: Martínez Sánchez
+Tipo Doc: T.I.
+Num Doc: CD567890 - 1681735403
+Roles: ['Solicitante', 'Recepción']</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Los datos del usuario aparecen correctamente en el modo edición</t>
+          <t>EXCEPTION</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>SI : ['birdwatcher22', 'Martín Andrés', 'Martínez Sánchez', 'Cédula de Extranjería', 'CD567890', True, ['Gestor 2', 'Recepción', 'Solicitante']] y ['birdwatcher22', 'Martín Andrés', 'Martínez Sánchez', 'Cédula de Extranjería', 'CD567890', True, ['Gestor 2', 'Recepción', 'Solicitante']] coinciden</t>
+          <t>list index out of range</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>PASSED</t>
+          <t>EXCEPTION</t>
         </is>
       </c>
     </row>
@@ -1539,11 +1539,11 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Nombres: Ana Isabel
-Apellidos: Ramírez González
-Tipo Doc: Pasaporte
-Num Doc: EF789012
-Roles: ['Recepción', 'Administrador']</t>
+          <t>Nombres: Santiago Alejandro
+Apellidos: Martínez Sánchez
+Tipo Doc: C.C.
+Num Doc: EF789012 - 1681735443
+Roles: ['Recepción', 'Gestor 1', 'Gestor 2']</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1578,11 +1578,11 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Nombres: Ana Isabel
-Apellidos: Ramírez González
-Tipo Doc: Pasaporte
-Num Doc: EF789012
-Roles: ['Recepción', 'Administrador']</t>
+          <t>Nombres: Santiago Alejandro
+Apellidos: Martínez Sánchez
+Tipo Doc: C.C.
+Num Doc: EF789012 - 1681735443
+Roles: ['Recepción', 'Gestor 1', 'Gestor 2']</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1592,7 +1592,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>SI : se encontró un resultado en Usuarios que coincide con [['butterflykisses44', 'Recepción Administrador']]</t>
+          <t>SI : se encontró un resultado en Usuarios que coincide con [['butterflykisses44 - 1681735443', 'Recepción Gestor 1 Gestor 2']]</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1617,11 +1617,11 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Nombres: Ana Isabel
-Apellidos: Ramírez González
-Tipo Doc: Pasaporte
-Num Doc: EF789012
-Roles: ['Recepción', 'Administrador']</t>
+          <t>Nombres: Santiago Alejandro
+Apellidos: Martínez Sánchez
+Tipo Doc: C.C.
+Num Doc: EF789012 - 1681735443
+Roles: ['Recepción', 'Gestor 1', 'Gestor 2']</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>SI : ['butterflykisses44', 'Ana Isabel', 'Ramírez González', 'Pasaporte', 'EF789012', True, ['Administrador', 'Recepción']] y ['butterflykisses44', 'Ana Isabel', 'Ramírez González', 'Pasaporte', 'EF789012', True, ['Administrador', 'Recepción']] coinciden</t>
+          <t>SI : ['butterflykisses44 - 1681735443', 'Santiago Alejandro', 'Martínez Sánchez', 'C.C.', 'EF789012 - 1681735443', True, ['Gestor 1', 'Gestor 2', 'Recepción']] y ['butterflykisses44 - 1681735443', 'Santiago Alejandro', 'Martínez Sánchez', 'C.C.', 'EF789012 - 1681735443', True, ['Gestor 1', 'Gestor 2', 'Recepción']] coinciden</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">

</xml_diff>